<commit_message>
committing in case i fuck up later
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="155">
   <si>
     <t>Pin</t>
   </si>
@@ -262,6 +262,225 @@
   </si>
   <si>
     <t>13.56Mhz Crystal</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>ADC2</t>
+  </si>
+  <si>
+    <t>ADC3</t>
+  </si>
+  <si>
+    <t>ADC4</t>
+  </si>
+  <si>
+    <t>ADC5</t>
+  </si>
+  <si>
+    <t>ADC6</t>
+  </si>
+  <si>
+    <t>ADC7</t>
+  </si>
+  <si>
+    <t>ADC8</t>
+  </si>
+  <si>
+    <t>SPI - MOSI</t>
+  </si>
+  <si>
+    <t>SPI - Chip Select</t>
+  </si>
+  <si>
+    <t>SPI - Clock</t>
+  </si>
+  <si>
+    <t>Port Name</t>
+  </si>
+  <si>
+    <t>PA12</t>
+  </si>
+  <si>
+    <t>AT91SAM7S64</t>
+  </si>
+  <si>
+    <t>PA13</t>
+  </si>
+  <si>
+    <t>PA14</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Eagle Wire Name</t>
+  </si>
+  <si>
+    <t>Analog to Digital Pin 1</t>
+  </si>
+  <si>
+    <t>Analog to Digital Pin 2</t>
+  </si>
+  <si>
+    <t>Analog to Digital Pin 3</t>
+  </si>
+  <si>
+    <t>Analog to Digital Pin 4</t>
+  </si>
+  <si>
+    <t>Analog to Digital Pin 5</t>
+  </si>
+  <si>
+    <t>Analog to Digital Pin 6</t>
+  </si>
+  <si>
+    <t>Analog to Digital Pin 7</t>
+  </si>
+  <si>
+    <t>Analog to Digital Pin 8</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>NCS</t>
+  </si>
+  <si>
+    <t>SPCK</t>
+  </si>
+  <si>
+    <t>SPI - MISO (MUST BE WIRED TO FPGA)</t>
+  </si>
+  <si>
+    <t>(MUST BE WIRED TO FPGA)</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>nprogram</t>
+  </si>
+  <si>
+    <t>cclk</t>
+  </si>
+  <si>
+    <t>din</t>
+  </si>
+  <si>
+    <t>dout</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>/PROGRAM</t>
+  </si>
+  <si>
+    <t>CCLK</t>
+  </si>
+  <si>
+    <t>P49</t>
+  </si>
+  <si>
+    <t>P51</t>
+  </si>
+  <si>
+    <t>P75</t>
+  </si>
+  <si>
+    <t>P73</t>
+  </si>
+  <si>
+    <t>P74</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>I/O (DIN, D0)</t>
+  </si>
+  <si>
+    <t>I/O (DOUT, BUSY)</t>
+  </si>
+  <si>
+    <t>tdi</t>
+  </si>
+  <si>
+    <t>tdo</t>
+  </si>
+  <si>
+    <t>tms</t>
+  </si>
+  <si>
+    <t>tck</t>
+  </si>
+  <si>
+    <t>P79</t>
+  </si>
+  <si>
+    <t>P77</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P99</t>
+  </si>
+  <si>
+    <t>TCK</t>
+  </si>
+  <si>
+    <t>TDO</t>
+  </si>
+  <si>
+    <t>TDI</t>
+  </si>
+  <si>
+    <t>TMS</t>
+  </si>
+  <si>
+    <t>FPGA_DONE</t>
+  </si>
+  <si>
+    <t>FPGA_NPROGRAM</t>
+  </si>
+  <si>
+    <t>FPGA_CCLK</t>
+  </si>
+  <si>
+    <t>FPGA_DIN</t>
+  </si>
+  <si>
+    <t>FPGA_DOUT</t>
+  </si>
+  <si>
+    <t>FPGA_TDI</t>
+  </si>
+  <si>
+    <t>FPGA_TDO</t>
+  </si>
+  <si>
+    <t>FPGA_TMS</t>
+  </si>
+  <si>
+    <t>FPGA_TCK</t>
+  </si>
+  <si>
+    <t>FPGA_INIT</t>
+  </si>
+  <si>
+    <t>P52</t>
+  </si>
+  <si>
+    <t>I/O (INIT)</t>
+  </si>
+  <si>
+    <t>init</t>
   </si>
 </sst>
 </file>
@@ -305,11 +524,91 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -318,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -327,10 +626,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -633,547 +972,933 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
     <col min="5" max="5" width="27.140625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="37.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="37.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="16"/>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="17">
         <v>3</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="17"/>
+      <c r="F5" s="7"/>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="17">
         <v>3</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="17"/>
+      <c r="F6" s="7"/>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="17">
         <v>3</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="17"/>
+      <c r="F7" s="7"/>
+      <c r="G7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>69</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="17">
         <v>3</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="17"/>
+      <c r="F8" s="7"/>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="17">
         <v>3</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="17"/>
+      <c r="F9" s="7"/>
+      <c r="G9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="17">
         <v>3</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="17"/>
+      <c r="F10" s="7"/>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="17">
         <v>3</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="17"/>
+      <c r="F11" s="7"/>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>72</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="17">
         <v>3</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="17"/>
+      <c r="F12" s="7"/>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="18">
         <v>1</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="18"/>
+      <c r="F13" s="10"/>
+      <c r="H13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="18">
         <v>4</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="18"/>
+      <c r="F14" s="10"/>
+      <c r="H14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" s="3">
+        <v>27</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="17">
         <v>4</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="17"/>
+      <c r="F15" s="7"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="17">
         <v>4</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="17"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="17"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>74</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="17">
         <v>0</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" t="s">
+      <c r="E17" s="17"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="17"/>
+      <c r="H17" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="17">
         <v>0</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="17"/>
+      <c r="H18" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
       <c r="B19" t="s">
         <v>68</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="17">
         <v>1</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="17"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="17"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="17">
         <v>6</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="17"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="17"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
       <c r="B21" t="s">
         <v>68</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="17">
         <v>4</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="17"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="3">
+        <v>22</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
         <v>68</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="17">
         <v>4</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="17"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H22" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" s="3">
+        <v>28</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="17">
         <v>5</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="17"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="17"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
       <c r="B24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="17">
         <v>1</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="17"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="17"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
       <c r="B25" t="s">
         <v>77</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="17">
         <v>1</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="17"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="17"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
       <c r="B26" t="s">
         <v>71</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="17">
         <v>1</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="17"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="17"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="17">
         <v>1</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="17"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
       <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="17">
         <v>1</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="17"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="17"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>49</v>
       </c>
       <c r="B29" t="s">
         <v>71</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="17">
         <v>1</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="17"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>51</v>
       </c>
       <c r="B30" t="s">
         <v>78</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="17">
         <v>4</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="17"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" s="3">
+        <v>21</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
       <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="17">
         <v>2</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="17"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="17"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>55</v>
       </c>
       <c r="B32" t="s">
         <v>68</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="17">
         <v>5</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="17"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="17"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
       <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="17">
         <v>5</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="17"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="17"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
       <c r="B34" t="s">
         <v>68</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="17">
         <v>5</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="17"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="8"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="20"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="17">
+        <v>3</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="20"/>
+      <c r="G36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="20"/>
+      <c r="G37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="17">
+        <v>2</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="20"/>
+      <c r="G38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="17">
+        <v>2</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="20"/>
+      <c r="G39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="17">
+        <v>2</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="20"/>
+      <c r="G40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" s="17">
+        <v>3</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="20"/>
+      <c r="G41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="20"/>
+      <c r="G42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" s="17">
+        <v>2</v>
+      </c>
+      <c r="E43" s="15"/>
+      <c r="F43" s="20"/>
+      <c r="G43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>141</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="20"/>
+      <c r="G44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="23"/>
+      <c r="G45" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more stuff to prevent confusion later
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G41" sqref="A41:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
backing up, better safe than sorry
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="160">
   <si>
     <t>Pin</t>
   </si>
@@ -481,23 +481,31 @@
   </si>
   <si>
     <t>init</t>
+  </si>
+  <si>
+    <t>VCCAUX</t>
+  </si>
+  <si>
+    <t>P100</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P76</t>
+  </si>
+  <si>
+    <t>P48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,17 +519,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -613,20 +616,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,10 +636,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -654,9 +651,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -670,9 +664,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -974,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G41" sqref="A41:G41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +977,7 @@
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11" style="2" customWidth="1"/>
     <col min="5" max="5" width="27.140625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
@@ -993,23 +987,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="12" t="s">
         <v>100</v>
       </c>
       <c r="H3" t="s">
@@ -1026,23 +1020,23 @@
       <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="13"/>
       <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="11" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1053,22 +1047,22 @@
       <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="14">
         <v>3</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="6"/>
       <c r="G5" t="s">
         <v>82</v>
       </c>
       <c r="H5" t="s">
         <v>101</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1077,22 +1071,22 @@
       <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="14">
         <v>3</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="6"/>
       <c r="G6" t="s">
         <v>83</v>
       </c>
       <c r="H6" t="s">
         <v>102</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1101,22 +1095,22 @@
       <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>3</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="6"/>
       <c r="G7" t="s">
         <v>84</v>
       </c>
       <c r="H7" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1125,22 +1119,22 @@
       <c r="B8" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="14">
         <v>3</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="6"/>
       <c r="G8" t="s">
         <v>85</v>
       </c>
       <c r="H8" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1149,22 +1143,22 @@
       <c r="B9" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="14">
         <v>3</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="6"/>
       <c r="G9" t="s">
         <v>86</v>
       </c>
       <c r="H9" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1173,22 +1167,22 @@
       <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="14">
         <v>3</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="7"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="6"/>
       <c r="G10" t="s">
         <v>87</v>
       </c>
       <c r="H10" t="s">
         <v>106</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1197,22 +1191,22 @@
       <c r="B11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="14">
         <v>3</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="6"/>
       <c r="G11" t="s">
         <v>88</v>
       </c>
       <c r="H11" t="s">
         <v>107</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1221,66 +1215,66 @@
       <c r="B12" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="14">
         <v>3</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="6"/>
       <c r="G12" t="s">
         <v>89</v>
       </c>
       <c r="H12" t="s">
         <v>108</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="14">
         <v>1</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="10"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="16"/>
       <c r="H13" t="s">
         <v>113</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="14">
         <v>4</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="16"/>
       <c r="H14" t="s">
         <v>112</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>27</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1291,16 +1285,16 @@
       <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="14">
         <v>4</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="7"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="6"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1309,17 +1303,17 @@
       <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="14">
         <v>4</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="17"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="14"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1328,22 +1322,22 @@
       <c r="B17" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="14">
         <v>0</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="17"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="14"/>
       <c r="H17" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1354,22 +1348,22 @@
       <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="14">
         <v>0</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="17"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="14"/>
       <c r="H18" t="s">
         <v>81</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1380,17 +1374,17 @@
       <c r="B19" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="14">
         <v>1</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="17"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="14"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1399,17 +1393,17 @@
       <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="14">
         <v>6</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="17"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="14"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1418,24 +1412,24 @@
       <c r="B21" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="14">
         <v>4</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="17" t="s">
+      <c r="E21" s="14"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="14" t="s">
         <v>109</v>
       </c>
       <c r="H21" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>22</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="2" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1446,24 +1440,24 @@
       <c r="B22" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="14">
         <v>4</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="17" t="s">
+      <c r="E22" s="14"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="14" t="s">
         <v>110</v>
       </c>
       <c r="H22" t="s">
         <v>91</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>28</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="2" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1474,17 +1468,17 @@
       <c r="B23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="14">
         <v>5</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="17"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="14"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1493,17 +1487,17 @@
       <c r="B24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="14">
         <v>1</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="17"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="14"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1512,17 +1506,17 @@
       <c r="B25" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="14">
         <v>1</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="17"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="14"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1531,17 +1525,17 @@
       <c r="B26" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="14">
         <v>1</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="17"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="14"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1550,17 +1544,17 @@
       <c r="B27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="14">
         <v>1</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="14"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1569,17 +1563,17 @@
       <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="14">
         <v>1</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="17"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1588,17 +1582,17 @@
       <c r="B29" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="14">
         <v>1</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="14"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1607,24 +1601,24 @@
       <c r="B30" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="14">
         <v>4</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="17" t="s">
+      <c r="E30" s="14"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="14" t="s">
         <v>111</v>
       </c>
       <c r="H30" t="s">
         <v>92</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <v>21</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="J30" s="2" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1635,17 +1629,17 @@
       <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="14">
         <v>2</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="17"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="14"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1654,17 +1648,17 @@
       <c r="B32" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="14">
         <v>5</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="17"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="14"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1673,17 +1667,17 @@
       <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="14">
         <v>5</v>
       </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="17"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="14"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1692,23 +1686,23 @@
       <c r="B34" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="14">
         <v>5</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="17"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="14"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C35" s="8"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="20"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1717,14 +1711,18 @@
       <c r="B36" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="14">
         <v>3</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="20"/>
+      <c r="E36" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="G36" t="s">
         <v>142</v>
       </c>
@@ -1736,14 +1734,18 @@
       <c r="B37" t="s">
         <v>120</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="20"/>
+      <c r="E37" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="G37" t="s">
         <v>143</v>
       </c>
@@ -1755,14 +1757,18 @@
       <c r="B38" t="s">
         <v>121</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="14">
         <v>2</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="20"/>
+      <c r="E38" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="16">
+        <v>2</v>
+      </c>
       <c r="G38" t="s">
         <v>144</v>
       </c>
@@ -1774,14 +1780,18 @@
       <c r="B39" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="14">
         <v>2</v>
       </c>
-      <c r="E39" s="15"/>
-      <c r="F39" s="20"/>
+      <c r="E39" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="F39" s="16">
+        <v>2</v>
+      </c>
       <c r="G39" t="s">
         <v>145</v>
       </c>
@@ -1790,17 +1800,21 @@
       <c r="A40" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="14">
         <v>2</v>
       </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="20"/>
+      <c r="E40" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="G40" t="s">
         <v>146</v>
       </c>
@@ -1812,14 +1826,18 @@
       <c r="B41" t="s">
         <v>153</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="14">
         <v>3</v>
       </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="20"/>
+      <c r="E41" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" s="16">
+        <v>2</v>
+      </c>
       <c r="G41" t="s">
         <v>151</v>
       </c>
@@ -1831,14 +1849,18 @@
       <c r="B42" t="s">
         <v>140</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="20"/>
+      <c r="E42" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="G42" t="s">
         <v>147</v>
       </c>
@@ -1850,14 +1872,18 @@
       <c r="B43" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="14">
         <v>2</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="20"/>
+      <c r="E43" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="G43" t="s">
         <v>148</v>
       </c>
@@ -1869,14 +1895,18 @@
       <c r="B44" t="s">
         <v>141</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="20"/>
+      <c r="E44" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="G44" t="s">
         <v>149</v>
       </c>
@@ -1888,14 +1918,18 @@
       <c r="B45" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="23"/>
+      <c r="E45" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>155</v>
+      </c>
       <c r="G45" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Initial pin configuration for the new fpga assigned! :) yay
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="236">
   <si>
     <t>Pin</t>
   </si>
@@ -658,6 +658,72 @@
   </si>
   <si>
     <t>input</t>
+  </si>
+  <si>
+    <t>P27</t>
+  </si>
+  <si>
+    <t>P28</t>
+  </si>
+  <si>
+    <t>P29</t>
+  </si>
+  <si>
+    <t>P30</t>
+  </si>
+  <si>
+    <t>P35</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P89</t>
+  </si>
+  <si>
+    <t>P90</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P64</t>
+  </si>
+  <si>
+    <t>P72</t>
+  </si>
+  <si>
+    <t>P65</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>P61</t>
+  </si>
+  <si>
+    <t>P59</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1302,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,8 +1428,12 @@
       <c r="E6" s="5">
         <v>3</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="F6" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
       <c r="H6" t="s">
         <v>82</v>
       </c>
@@ -1393,8 +1463,12 @@
       <c r="E7" s="5">
         <v>3</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="G7" s="7">
+        <v>2</v>
+      </c>
       <c r="H7" t="s">
         <v>83</v>
       </c>
@@ -1424,8 +1498,12 @@
       <c r="E8" s="5">
         <v>3</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2</v>
+      </c>
       <c r="H8" t="s">
         <v>84</v>
       </c>
@@ -1455,8 +1533,12 @@
       <c r="E9" s="5">
         <v>3</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="F9" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2</v>
+      </c>
       <c r="H9" t="s">
         <v>85</v>
       </c>
@@ -1486,8 +1568,12 @@
       <c r="E10" s="5">
         <v>3</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="F10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
       <c r="H10" t="s">
         <v>86</v>
       </c>
@@ -1517,8 +1603,12 @@
       <c r="E11" s="5">
         <v>3</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="F11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="7">
+        <v>2</v>
+      </c>
       <c r="H11" t="s">
         <v>87</v>
       </c>
@@ -1548,8 +1638,12 @@
       <c r="E12" s="5">
         <v>3</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2</v>
+      </c>
       <c r="H12" t="s">
         <v>88</v>
       </c>
@@ -1579,8 +1673,12 @@
       <c r="E13" s="5">
         <v>3</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="F13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2</v>
+      </c>
       <c r="H13" t="s">
         <v>89</v>
       </c>
@@ -1610,8 +1708,12 @@
       <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="G14" s="7">
+        <v>3</v>
+      </c>
       <c r="H14" t="s">
         <v>203</v>
       </c>
@@ -1641,8 +1743,12 @@
       <c r="E15" s="5">
         <v>4</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
       <c r="H15" t="s">
         <v>111</v>
       </c>
@@ -1672,8 +1778,12 @@
       <c r="E16" s="5">
         <v>4</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="F16" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3</v>
+      </c>
       <c r="H16" t="s">
         <v>207</v>
       </c>
@@ -1703,8 +1813,12 @@
       <c r="E17" s="5">
         <v>4</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="F17" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="G17" s="7">
+        <v>3</v>
+      </c>
       <c r="H17" s="2" t="s">
         <v>209</v>
       </c>
@@ -1734,8 +1848,12 @@
       <c r="E18" s="5">
         <v>0</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="F18" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
       <c r="H18" s="2" t="s">
         <v>211</v>
       </c>
@@ -1765,8 +1883,12 @@
       <c r="E19" s="5">
         <v>0</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
+      <c r="F19" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
       <c r="H19" s="2" t="s">
         <v>211</v>
       </c>
@@ -1796,8 +1918,12 @@
       <c r="E20" s="5">
         <v>1</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+      <c r="F20" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="G20" s="7">
+        <v>3</v>
+      </c>
       <c r="H20" s="2" t="s">
         <v>202</v>
       </c>
@@ -1827,8 +1953,12 @@
       <c r="E21" s="5">
         <v>6</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="F21" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
       <c r="H21" s="2" t="s">
         <v>200</v>
       </c>
@@ -1858,8 +1988,12 @@
       <c r="E22" s="5">
         <v>4</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
+      <c r="F22" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
       <c r="H22" s="2" t="s">
         <v>108</v>
       </c>
@@ -1889,8 +2023,12 @@
       <c r="E23" s="5">
         <v>4</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="F23" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>109</v>
       </c>
@@ -1920,8 +2058,12 @@
       <c r="E24" s="5">
         <v>5</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
+      <c r="F24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1</v>
+      </c>
       <c r="H24" s="2" t="s">
         <v>187</v>
       </c>
@@ -1951,8 +2093,12 @@
       <c r="E25" s="5">
         <v>1</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="F25" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="G25" s="7">
+        <v>3</v>
+      </c>
       <c r="H25" s="2" t="s">
         <v>189</v>
       </c>
@@ -1982,8 +2128,12 @@
       <c r="E26" s="5">
         <v>1</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="F26" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G26" s="7">
+        <v>3</v>
+      </c>
       <c r="H26" s="2" t="s">
         <v>190</v>
       </c>
@@ -2013,8 +2163,12 @@
       <c r="E27" s="5">
         <v>1</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="F27" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="G27" s="7">
+        <v>3</v>
+      </c>
       <c r="H27" s="2" t="s">
         <v>191</v>
       </c>
@@ -2044,8 +2198,12 @@
       <c r="E28" s="5">
         <v>1</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
+      <c r="F28" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="G28" s="7">
+        <v>3</v>
+      </c>
       <c r="H28" s="2" t="s">
         <v>192</v>
       </c>
@@ -2075,8 +2233,12 @@
       <c r="E29" s="5">
         <v>1</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
+      <c r="F29" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G29" s="7">
+        <v>3</v>
+      </c>
       <c r="H29" s="2" t="s">
         <v>193</v>
       </c>
@@ -2106,8 +2268,12 @@
       <c r="E30" s="5">
         <v>1</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
+      <c r="F30" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="G30" s="7">
+        <v>3</v>
+      </c>
       <c r="H30" s="2" t="s">
         <v>194</v>
       </c>
@@ -2137,8 +2303,12 @@
       <c r="E31" s="5">
         <v>4</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="F31" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="7">
+        <v>1</v>
+      </c>
       <c r="H31" s="2" t="s">
         <v>110</v>
       </c>
@@ -2168,8 +2338,12 @@
       <c r="E32" s="5">
         <v>2</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
+      <c r="F32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
       <c r="H32" s="2" t="s">
         <v>182</v>
       </c>
@@ -2199,8 +2373,12 @@
       <c r="E33" s="5">
         <v>5</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
+      <c r="F33" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1</v>
+      </c>
       <c r="H33" s="2" t="s">
         <v>181</v>
       </c>
@@ -2230,8 +2408,12 @@
       <c r="E34" s="5">
         <v>5</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
+      <c r="F34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
       <c r="H34" s="2" t="s">
         <v>180</v>
       </c>
@@ -2261,8 +2443,12 @@
       <c r="E35" s="5">
         <v>5</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
+      <c r="F35" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="G35" s="7">
+        <v>1</v>
+      </c>
       <c r="H35" s="2" t="s">
         <v>179</v>
       </c>

</xml_diff>

<commit_message>
New and improved pin assignment, next revision contains matching code
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -696,9 +696,6 @@
     <t>P64</t>
   </si>
   <si>
-    <t>P72</t>
-  </si>
-  <si>
     <t>P65</t>
   </si>
   <si>
@@ -724,6 +721,9 @@
   </si>
   <si>
     <t>P59</t>
+  </si>
+  <si>
+    <t>P70</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1302,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,7 +1709,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G14" s="7">
         <v>3</v>
@@ -1744,7 +1744,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
       <c r="G15" s="7">
         <v>1</v>
@@ -1919,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="G20" s="7">
         <v>3</v>
@@ -1989,7 +1989,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="G22" s="7">
         <v>1</v>
@@ -2024,7 +2024,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G23" s="7">
         <v>1</v>
@@ -2059,10 +2059,10 @@
         <v>5</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G24" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>187</v>
@@ -2094,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="G25" s="7">
         <v>3</v>
@@ -2129,7 +2129,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G26" s="7">
         <v>3</v>
@@ -2164,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G27" s="7">
         <v>3</v>
@@ -2199,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G28" s="7">
         <v>3</v>
@@ -2234,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G29" s="7">
         <v>3</v>
@@ -2269,7 +2269,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G30" s="7">
         <v>3</v>
@@ -2304,10 +2304,10 @@
         <v>4</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G31" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>110</v>
@@ -2374,7 +2374,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G33" s="7">
         <v>1</v>
@@ -2444,7 +2444,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G35" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
Updated pins with uart in the excel sheet
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="254">
   <si>
     <t>Pin</t>
   </si>
@@ -724,6 +724,60 @@
   </si>
   <si>
     <t>P70</t>
+  </si>
+  <si>
+    <t>uart_rx</t>
+  </si>
+  <si>
+    <t>IO_L08P_2/GCLK14</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>UART - RX</t>
+  </si>
+  <si>
+    <t>uart_tx</t>
+  </si>
+  <si>
+    <t>IO_L08N_2/GCLK15</t>
+  </si>
+  <si>
+    <t>P41</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UART - TX</t>
+  </si>
+  <si>
+    <t>uart_io1</t>
+  </si>
+  <si>
+    <t>input/output</t>
+  </si>
+  <si>
+    <t>UART_IO1</t>
+  </si>
+  <si>
+    <t>UART - IO1</t>
+  </si>
+  <si>
+    <t>IO_L09P_2/GCLK0</t>
+  </si>
+  <si>
+    <t>uart_io2</t>
+  </si>
+  <si>
+    <t>IO_L09N_2/GCLK1</t>
+  </si>
+  <si>
+    <t>UART_IO2</t>
+  </si>
+  <si>
+    <t>UART - IO2</t>
   </si>
 </sst>
 </file>
@@ -807,7 +861,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -920,6 +974,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -927,7 +994,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -994,6 +1061,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1299,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,419 +2538,507 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
+      <c r="A36" t="s">
+        <v>236</v>
+      </c>
+      <c r="B36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C36" t="s">
+        <v>213</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="7">
+        <v>2</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I36" t="s">
+        <v>239</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>240</v>
       </c>
       <c r="B37" t="s">
-        <v>118</v>
+        <v>241</v>
       </c>
       <c r="C37" t="s">
-        <v>126</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E37" s="5">
-        <v>3</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="H37" t="s">
-        <v>141</v>
+        <v>212</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G37" s="7">
+        <v>2</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="I37" t="s">
-        <v>166</v>
-      </c>
-      <c r="J37" s="1">
-        <v>37</v>
+        <v>244</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>245</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>249</v>
       </c>
       <c r="C38" t="s">
-        <v>126</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="H38" t="s">
-        <v>142</v>
+        <v>246</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="7">
+        <v>2</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="I38" t="s">
-        <v>165</v>
-      </c>
-      <c r="J38" s="1">
-        <v>38</v>
+        <v>248</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>250</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>251</v>
       </c>
       <c r="C39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E39" s="5">
-        <v>2</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>19</v>
+        <v>246</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="G39" s="7">
         <v>2</v>
       </c>
-      <c r="H39" t="s">
-        <v>143</v>
+      <c r="H39" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="I39" t="s">
-        <v>170</v>
-      </c>
-      <c r="J39" s="1">
-        <v>41</v>
+        <v>253</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" t="s">
-        <v>126</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E40" s="5">
-        <v>2</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="7">
-        <v>2</v>
-      </c>
-      <c r="H40" t="s">
-        <v>144</v>
-      </c>
-      <c r="I40" t="s">
-        <v>169</v>
-      </c>
-      <c r="J40" s="1">
-        <v>42</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>128</v>
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>118</v>
       </c>
       <c r="C41" t="s">
         <v>126</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E41" s="5">
-        <v>2</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>126</v>
+        <v>3</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="H41" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J41" s="1">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
         <v>126</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="5">
-        <v>3</v>
+        <v>122</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G42" s="7">
-        <v>2</v>
+        <v>155</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="H42" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J42" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
         <v>126</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="E43" s="5">
+        <v>2</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>154</v>
+        <v>19</v>
+      </c>
+      <c r="G43" s="7">
+        <v>2</v>
       </c>
       <c r="H43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I43" t="s">
-        <v>171</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>126</v>
+        <v>170</v>
+      </c>
+      <c r="J43" s="1">
+        <v>41</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
         <v>126</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E44" s="5">
         <v>2</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>154</v>
+        <v>122</v>
+      </c>
+      <c r="G44" s="7">
+        <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I44" t="s">
-        <v>172</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>126</v>
+        <v>169</v>
+      </c>
+      <c r="J44" s="1">
+        <v>42</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>131</v>
-      </c>
-      <c r="B45" t="s">
-        <v>140</v>
+        <v>117</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C45" t="s">
         <v>126</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>154</v>
+        <v>125</v>
+      </c>
+      <c r="E45" s="5">
+        <v>2</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="H45" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I45" t="s">
-        <v>173</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>126</v>
+        <v>168</v>
+      </c>
+      <c r="J45" s="1">
+        <v>52</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="5">
+        <v>3</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G46" s="7">
+        <v>2</v>
+      </c>
+      <c r="H46" t="s">
+        <v>150</v>
+      </c>
+      <c r="I46" t="s">
+        <v>167</v>
+      </c>
+      <c r="J46" s="1">
+        <v>36</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H47" t="s">
+        <v>146</v>
+      </c>
+      <c r="I47" t="s">
+        <v>171</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" s="5">
+        <v>2</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H48" t="s">
+        <v>147</v>
+      </c>
+      <c r="I48" t="s">
+        <v>172</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H49" t="s">
+        <v>148</v>
+      </c>
+      <c r="I49" t="s">
+        <v>173</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>132</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B50" t="s">
         <v>137</v>
       </c>
-      <c r="C46" t="s">
-        <v>126</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="C50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F46" s="6" t="s">
+      <c r="E50" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="G50" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H50" t="s">
         <v>149</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I50" t="s">
         <v>174</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
+      <c r="J50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
@@ -2887,8 +3050,60 @@
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update fpga pins with uart
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -618,9 +618,6 @@
     <t>Global Clock Buffer</t>
   </si>
   <si>
-    <t>N$55</t>
-  </si>
-  <si>
     <t>Test Point</t>
   </si>
   <si>
@@ -651,9 +648,6 @@
     <t>ADC Enable</t>
   </si>
   <si>
-    <t>N$5</t>
-  </si>
-  <si>
     <t>output</t>
   </si>
   <si>
@@ -778,6 +772,12 @@
   </si>
   <si>
     <t>UART - IO2</t>
+  </si>
+  <si>
+    <t>1356_CRYSTAL</t>
+  </si>
+  <si>
+    <t>DBG</t>
   </si>
 </sst>
 </file>
@@ -1376,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,7 +1451,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
@@ -1495,7 +1495,7 @@
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
@@ -1504,7 +1504,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G6" s="7">
         <v>2</v>
@@ -1530,7 +1530,7 @@
         <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>7</v>
@@ -1539,7 +1539,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G7" s="7">
         <v>2</v>
@@ -1565,7 +1565,7 @@
         <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>9</v>
@@ -1574,7 +1574,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G8" s="7">
         <v>2</v>
@@ -1600,7 +1600,7 @@
         <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
@@ -1609,7 +1609,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G9" s="7">
         <v>2</v>
@@ -1635,7 +1635,7 @@
         <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>16</v>
@@ -1670,7 +1670,7 @@
         <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>17</v>
@@ -1705,7 +1705,7 @@
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>18</v>
@@ -1714,7 +1714,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G12" s="7">
         <v>2</v>
@@ -1740,7 +1740,7 @@
         <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>19</v>
@@ -1775,7 +1775,7 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>62</v>
@@ -1784,16 +1784,16 @@
         <v>1</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G14" s="7">
         <v>3</v>
       </c>
       <c r="H14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I14" t="s">
         <v>203</v>
-      </c>
-      <c r="I14" t="s">
-        <v>204</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>126</v>
@@ -1810,7 +1810,7 @@
         <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>64</v>
@@ -1845,7 +1845,7 @@
         <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>21</v>
@@ -1854,16 +1854,16 @@
         <v>4</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G16" s="7">
         <v>3</v>
       </c>
       <c r="H16" t="s">
+        <v>206</v>
+      </c>
+      <c r="I16" t="s">
         <v>207</v>
-      </c>
-      <c r="I16" t="s">
-        <v>208</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>126</v>
@@ -1880,7 +1880,7 @@
         <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>24</v>
@@ -1889,16 +1889,16 @@
         <v>4</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G17" s="7">
         <v>3</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I17" t="s">
         <v>209</v>
-      </c>
-      <c r="I17" t="s">
-        <v>210</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>126</v>
@@ -1915,7 +1915,7 @@
         <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>26</v>
@@ -1924,13 +1924,13 @@
         <v>0</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G18" s="7">
         <v>0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="I18" t="s">
         <v>81</v>
@@ -1950,7 +1950,7 @@
         <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>28</v>
@@ -1959,13 +1959,13 @@
         <v>0</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G19" s="7">
         <v>0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="I19" t="s">
         <v>81</v>
@@ -1985,7 +1985,7 @@
         <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>30</v>
@@ -1994,16 +1994,16 @@
         <v>1</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G20" s="7">
         <v>3</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>126</v>
@@ -2020,7 +2020,7 @@
         <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>32</v>
@@ -2029,16 +2029,16 @@
         <v>6</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G21" s="7">
         <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I21" t="s">
         <v>200</v>
-      </c>
-      <c r="I21" t="s">
-        <v>201</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>126</v>
@@ -2055,7 +2055,7 @@
         <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>34</v>
@@ -2064,7 +2064,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G22" s="7">
         <v>1</v>
@@ -2090,7 +2090,7 @@
         <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>36</v>
@@ -2099,7 +2099,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G23" s="7">
         <v>1</v>
@@ -2125,7 +2125,7 @@
         <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>38</v>
@@ -2160,7 +2160,7 @@
         <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>40</v>
@@ -2169,7 +2169,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G25" s="7">
         <v>3</v>
@@ -2195,7 +2195,7 @@
         <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>42</v>
@@ -2204,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G26" s="7">
         <v>3</v>
@@ -2230,7 +2230,7 @@
         <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>44</v>
@@ -2239,7 +2239,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G27" s="7">
         <v>3</v>
@@ -2265,7 +2265,7 @@
         <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>46</v>
@@ -2274,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G28" s="7">
         <v>3</v>
@@ -2300,7 +2300,7 @@
         <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>48</v>
@@ -2309,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G29" s="7">
         <v>3</v>
@@ -2335,7 +2335,7 @@
         <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>50</v>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G30" s="7">
         <v>3</v>
@@ -2370,7 +2370,7 @@
         <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>52</v>
@@ -2405,7 +2405,7 @@
         <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>54</v>
@@ -2440,7 +2440,7 @@
         <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>56</v>
@@ -2449,7 +2449,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G33" s="7">
         <v>1</v>
@@ -2475,7 +2475,7 @@
         <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>58</v>
@@ -2510,7 +2510,7 @@
         <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>60</v>
@@ -2519,7 +2519,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G35" s="7">
         <v>1</v>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B36" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D36" s="35" t="s">
         <v>126</v>
@@ -2560,10 +2560,10 @@
         <v>2</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I36" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>126</v>
@@ -2574,31 +2574,31 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" t="s">
+        <v>210</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="B37" t="s">
-        <v>241</v>
-      </c>
-      <c r="C37" t="s">
-        <v>212</v>
-      </c>
-      <c r="D37" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E37" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="G37" s="7">
         <v>2</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I37" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>126</v>
@@ -2609,13 +2609,13 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B38" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C38" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D38" s="35" t="s">
         <v>126</v>
@@ -2630,10 +2630,10 @@
         <v>2</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>126</v>
@@ -2644,13 +2644,13 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B39" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C39" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D39" s="35" t="s">
         <v>126</v>
@@ -2665,10 +2665,10 @@
         <v>2</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I39" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Updated Datasheet, Excel file, FPGA and FPGA_EXPERIMENTAL code with the corrected Spartan-3 ucf/pin config
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="251">
   <si>
     <t>Pin</t>
   </si>
@@ -24,9 +24,6 @@
     <t>XC2S30-5VQG100C - Spartan-II</t>
   </si>
   <si>
-    <t>XC3S50A-VQ100 - Spartan-3A</t>
-  </si>
-  <si>
     <t>Function Pin</t>
   </si>
   <si>
@@ -480,15 +477,9 @@
     <t>init</t>
   </si>
   <si>
-    <t>VCCAUX</t>
-  </si>
-  <si>
     <t>P100</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>P76</t>
   </si>
   <si>
@@ -660,9 +651,6 @@
     <t>P28</t>
   </si>
   <si>
-    <t>P29</t>
-  </si>
-  <si>
     <t>P30</t>
   </si>
   <si>
@@ -672,9 +660,6 @@
     <t>P5</t>
   </si>
   <si>
-    <t>P3</t>
-  </si>
-  <si>
     <t>P4</t>
   </si>
   <si>
@@ -684,42 +669,18 @@
     <t>P90</t>
   </si>
   <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>P64</t>
-  </si>
-  <si>
-    <t>P65</t>
-  </si>
-  <si>
     <t>P9</t>
   </si>
   <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>P13</t>
-  </si>
-  <si>
     <t>P15</t>
   </si>
   <si>
-    <t>P16</t>
-  </si>
-  <si>
     <t>P61</t>
   </si>
   <si>
     <t>P59</t>
   </si>
   <si>
-    <t>P70</t>
-  </si>
-  <si>
     <t>uart_rx</t>
   </si>
   <si>
@@ -738,9 +699,6 @@
     <t>IO_L08N_2/GCLK15</t>
   </si>
   <si>
-    <t>P41</t>
-  </si>
-  <si>
     <t>TX</t>
   </si>
   <si>
@@ -778,6 +736,39 @@
   </si>
   <si>
     <t>DBG</t>
+  </si>
+  <si>
+    <t>XC3S50-5VQ100 - Spartan-3</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>P72</t>
+  </si>
+  <si>
+    <t>P37</t>
+  </si>
+  <si>
+    <t>P67</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>P42</t>
+  </si>
+  <si>
+    <t>P78</t>
   </si>
 </sst>
 </file>
@@ -994,7 +985,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1009,7 +1000,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1376,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,1714 +1386,1714 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="16"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23" t="s">
+      <c r="J3" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="25"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="28" t="s">
+      <c r="E4" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="30" t="s">
+      <c r="G4" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="28"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="31" t="s">
-        <v>93</v>
+      <c r="K4" s="30" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="E6" s="5">
         <v>3</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="G6" s="7">
-        <v>2</v>
+      <c r="F6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="6">
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="E7" s="5">
         <v>3</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="G7" s="7">
-        <v>2</v>
+      <c r="F7" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="E8" s="5">
         <v>3</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="G8" s="7">
-        <v>2</v>
+      <c r="F8" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G8" s="6">
+        <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="5">
         <v>3</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="G9" s="7">
-        <v>2</v>
+      <c r="F9" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="5">
         <v>3</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="7">
-        <v>2</v>
+      <c r="F10" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="5">
         <v>3</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="7">
-        <v>2</v>
+      <c r="F11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="6">
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="5">
         <v>3</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G12" s="7">
-        <v>2</v>
+      <c r="F12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="6">
+        <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="5">
         <v>3</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="7">
-        <v>2</v>
+      <c r="F13" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" s="6">
+        <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="G14" s="7">
-        <v>3</v>
+      <c r="F14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="6">
+        <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>210</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="E15" s="5">
         <v>4</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="7">
-        <v>1</v>
+      <c r="F15" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G15" s="6">
+        <v>2</v>
       </c>
       <c r="H15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" t="s">
         <v>111</v>
-      </c>
-      <c r="I15" t="s">
-        <v>112</v>
       </c>
       <c r="J15" s="1">
         <v>27</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" t="s">
-        <v>210</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E16" s="5">
         <v>4</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="G16" s="7">
-        <v>3</v>
+      <c r="F16" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G16" s="6">
+        <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" t="s">
-        <v>210</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E17" s="5">
         <v>4</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="G17" s="7">
-        <v>3</v>
+      <c r="F17" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" s="6">
+        <v>7</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I17" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" t="s">
-        <v>211</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="G18" s="7">
+      <c r="F18" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="G18" s="6">
         <v>0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>211</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="G19" s="7">
+      <c r="F19" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="G19" s="6">
         <v>0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="I19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
+        <v>208</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>211</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="G20" s="7">
-        <v>3</v>
+      <c r="F20" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="G20" s="6">
+        <v>5</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="I20" t="s">
         <v>201</v>
       </c>
-      <c r="I20" t="s">
-        <v>204</v>
-      </c>
       <c r="J20" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" t="s">
-        <v>210</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E21" s="5">
         <v>6</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="G21" s="7">
-        <v>1</v>
+      <c r="F21" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="G21" s="6">
+        <v>2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="I21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" t="s">
-        <v>211</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="E22" s="5">
         <v>4</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="G22" s="7">
-        <v>1</v>
+      <c r="F22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="6">
+        <v>2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J22" s="1">
         <v>22</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>208</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" t="s">
-        <v>211</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="E23" s="5">
         <v>4</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="G23" s="7">
-        <v>1</v>
+      <c r="F23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="6">
+        <v>4</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J23" s="1">
         <v>28</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>208</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" t="s">
-        <v>211</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="E24" s="5">
         <v>5</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="7">
-        <v>0</v>
+      <c r="F24" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I24" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J24" s="1">
         <v>34</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" t="s">
-        <v>210</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="G25" s="7">
-        <v>3</v>
+      <c r="F25" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G25" s="6">
+        <v>7</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I25" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>207</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" t="s">
-        <v>210</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="G26" s="7">
-        <v>3</v>
+      <c r="F26" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="G26" s="6">
+        <v>7</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I26" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>207</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" t="s">
-        <v>210</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="G27" s="7">
-        <v>3</v>
+      <c r="F27" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G27" s="6">
+        <v>6</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
+        <v>207</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" t="s">
-        <v>210</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="G28" s="7">
-        <v>3</v>
+      <c r="F28" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="G28" s="6">
+        <v>6</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I28" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>207</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>210</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="E29" s="5">
         <v>1</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G29" s="7">
-        <v>3</v>
+      <c r="F29" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="G29" s="6">
+        <v>6</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I29" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
+        <v>207</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" t="s">
-        <v>210</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="G30" s="7">
-        <v>3</v>
+      <c r="F30" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="G30" s="6">
+        <v>6</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="I30" t="s">
         <v>194</v>
       </c>
-      <c r="I30" t="s">
-        <v>197</v>
-      </c>
       <c r="J30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>211</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="E31" s="5">
         <v>4</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="7">
-        <v>0</v>
+      <c r="F31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="6">
+        <v>1</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J31" s="1">
         <v>21</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>207</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" t="s">
-        <v>210</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="E32" s="5">
         <v>2</v>
       </c>
-      <c r="F32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" s="7">
-        <v>1</v>
+      <c r="F32" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="6">
+        <v>3</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I32" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J32" s="1">
         <v>19</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>207</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" t="s">
-        <v>210</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="E33" s="5">
         <v>5</v>
       </c>
-      <c r="F33" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="G33" s="7">
-        <v>1</v>
+      <c r="F33" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G33" s="6">
+        <v>3</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J33" s="1">
         <v>10</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>208</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" t="s">
-        <v>211</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="E34" s="5">
         <v>5</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="7">
-        <v>1</v>
+      <c r="F34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="6">
+        <v>3</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I34" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J34" s="1">
         <v>9</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>207</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" t="s">
-        <v>210</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="E35" s="5">
         <v>5</v>
       </c>
-      <c r="F35" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="G35" s="7">
-        <v>1</v>
+      <c r="F35" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G35" s="6">
+        <v>3</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I35" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J35" s="1">
         <v>20</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="B36" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C36" t="s">
-        <v>211</v>
-      </c>
-      <c r="D36" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E36" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" s="7">
-        <v>2</v>
+        <v>208</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36" s="6">
+        <v>4</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="I36" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B37" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C37" t="s">
-        <v>210</v>
-      </c>
-      <c r="D37" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E37" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="G37" s="7">
-        <v>2</v>
+        <v>207</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G37" s="6">
+        <v>4</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="I37" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="B38" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C38" t="s">
-        <v>244</v>
-      </c>
-      <c r="D38" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E38" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G38" s="7">
-        <v>2</v>
+        <v>230</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="6">
+        <v>4</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="I38" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B39" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C39" t="s">
-        <v>244</v>
-      </c>
-      <c r="D39" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E39" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" s="7">
-        <v>2</v>
+        <v>230</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="6">
+        <v>3</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="I39" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E41" s="5">
         <v>3</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>154</v>
+      <c r="F41" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="H41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J41" s="1">
         <v>37</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>154</v>
+        <v>125</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="H42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I42" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J42" s="1">
         <v>38</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E43" s="5">
         <v>2</v>
       </c>
-      <c r="F43" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G43" s="7">
-        <v>2</v>
+      <c r="F43" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="H43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I43" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J43" s="1">
         <v>41</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E44" s="5">
         <v>2</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G44" s="7">
-        <v>2</v>
+      <c r="F44" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G44" s="6">
+        <v>4</v>
       </c>
       <c r="H44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I44" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J44" s="1">
         <v>42</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E45" s="5">
         <v>2</v>
       </c>
-      <c r="F45" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>126</v>
+      <c r="F45" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" s="7">
+        <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I45" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J45" s="1">
         <v>52</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E46" s="5">
         <v>3</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G46" s="7">
-        <v>2</v>
+      <c r="F46" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="G46" s="6">
+        <v>4</v>
       </c>
       <c r="H46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I46" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J46" s="1">
         <v>36</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>154</v>
+        <v>125</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="H47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I47" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E48" s="5">
         <v>2</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G48" s="6" t="s">
+      <c r="F48" s="8" t="s">
         <v>154</v>
       </c>
+      <c r="G48" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="H48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I48" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>154</v>
+        <v>125</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="H49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I49" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C50" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>154</v>
+        <v>125</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="H50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I50" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="10"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the FPGA pin configuration for the stm32-prox board to use the new Spartan-3 pin configuration
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -465,9 +465,6 @@
     <t>FPGA_TCK</t>
   </si>
   <si>
-    <t>FPGA_INIT</t>
-  </si>
-  <si>
     <t>P52</t>
   </si>
   <si>
@@ -769,6 +766,9 @@
   </si>
   <si>
     <t>P78</t>
+  </si>
+  <si>
+    <t>FPGA_NINIT</t>
   </si>
 </sst>
 </file>
@@ -1366,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="23" t="s">
@@ -1441,7 +1441,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>0</v>
@@ -1485,7 +1485,7 @@
         <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>4</v>
@@ -1520,7 +1520,7 @@
         <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>6</v>
@@ -1529,7 +1529,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G7" s="6">
         <v>6</v>
@@ -1555,7 +1555,7 @@
         <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
@@ -1564,7 +1564,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G8" s="6">
         <v>5</v>
@@ -1590,7 +1590,7 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
@@ -1599,7 +1599,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G9" s="6">
         <v>5</v>
@@ -1625,7 +1625,7 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
@@ -1634,7 +1634,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G10" s="6">
         <v>5</v>
@@ -1660,7 +1660,7 @@
         <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>16</v>
@@ -1695,7 +1695,7 @@
         <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>17</v>
@@ -1730,7 +1730,7 @@
         <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>18</v>
@@ -1739,7 +1739,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G13" s="6">
         <v>5</v>
@@ -1765,7 +1765,7 @@
         <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>61</v>
@@ -1780,10 +1780,10 @@
         <v>5</v>
       </c>
       <c r="H14" t="s">
+        <v>198</v>
+      </c>
+      <c r="I14" t="s">
         <v>199</v>
-      </c>
-      <c r="I14" t="s">
-        <v>200</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>125</v>
@@ -1800,7 +1800,7 @@
         <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>63</v>
@@ -1809,7 +1809,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G15" s="6">
         <v>2</v>
@@ -1835,7 +1835,7 @@
         <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>20</v>
@@ -1844,16 +1844,16 @@
         <v>4</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G16" s="6">
         <v>7</v>
       </c>
       <c r="H16" t="s">
+        <v>202</v>
+      </c>
+      <c r="I16" t="s">
         <v>203</v>
-      </c>
-      <c r="I16" t="s">
-        <v>204</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>125</v>
@@ -1870,7 +1870,7 @@
         <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>23</v>
@@ -1879,16 +1879,16 @@
         <v>4</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G17" s="6">
         <v>7</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I17" t="s">
         <v>205</v>
-      </c>
-      <c r="I17" t="s">
-        <v>206</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>125</v>
@@ -1905,7 +1905,7 @@
         <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>25</v>
@@ -1914,13 +1914,13 @@
         <v>0</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G18" s="6">
         <v>0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I18" t="s">
         <v>80</v>
@@ -1940,7 +1940,7 @@
         <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>27</v>
@@ -1949,13 +1949,13 @@
         <v>0</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G19" s="6">
         <v>0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I19" t="s">
         <v>80</v>
@@ -1975,7 +1975,7 @@
         <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>29</v>
@@ -1984,16 +1984,16 @@
         <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G20" s="6">
         <v>5</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>125</v>
@@ -2010,7 +2010,7 @@
         <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>31</v>
@@ -2019,16 +2019,16 @@
         <v>6</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G21" s="6">
         <v>2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>125</v>
@@ -2045,7 +2045,7 @@
         <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>33</v>
@@ -2080,7 +2080,7 @@
         <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>35</v>
@@ -2115,7 +2115,7 @@
         <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>37</v>
@@ -2130,16 +2130,16 @@
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J24" s="1">
         <v>34</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2150,7 +2150,7 @@
         <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>39</v>
@@ -2159,16 +2159,16 @@
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G25" s="6">
         <v>7</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>125</v>
@@ -2185,7 +2185,7 @@
         <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>41</v>
@@ -2194,16 +2194,16 @@
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G26" s="6">
         <v>7</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>125</v>
@@ -2220,7 +2220,7 @@
         <v>70</v>
       </c>
       <c r="C27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>43</v>
@@ -2229,16 +2229,16 @@
         <v>1</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G27" s="6">
         <v>6</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>125</v>
@@ -2255,7 +2255,7 @@
         <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>45</v>
@@ -2264,16 +2264,16 @@
         <v>1</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G28" s="6">
         <v>6</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>125</v>
@@ -2290,7 +2290,7 @@
         <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>47</v>
@@ -2299,16 +2299,16 @@
         <v>1</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G29" s="6">
         <v>6</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>125</v>
@@ -2325,7 +2325,7 @@
         <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>49</v>
@@ -2334,16 +2334,16 @@
         <v>1</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G30" s="6">
         <v>6</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>125</v>
@@ -2360,7 +2360,7 @@
         <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>51</v>
@@ -2395,7 +2395,7 @@
         <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>53</v>
@@ -2410,16 +2410,16 @@
         <v>3</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J32" s="1">
         <v>19</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>55</v>
@@ -2439,22 +2439,22 @@
         <v>5</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G33" s="6">
         <v>3</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J33" s="1">
         <v>10</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
         <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>57</v>
@@ -2480,16 +2480,16 @@
         <v>3</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J34" s="1">
         <v>9</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>59</v>
@@ -2509,33 +2509,33 @@
         <v>5</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G35" s="6">
         <v>3</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J35" s="1">
         <v>20</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>220</v>
+      </c>
+      <c r="B36" t="s">
         <v>221</v>
       </c>
-      <c r="B36" t="s">
-        <v>222</v>
-      </c>
       <c r="C36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D36" s="34" t="s">
         <v>125</v>
@@ -2550,10 +2550,10 @@
         <v>4</v>
       </c>
       <c r="H36" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I36" t="s">
         <v>223</v>
-      </c>
-      <c r="I36" t="s">
-        <v>224</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>125</v>
@@ -2564,13 +2564,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>224</v>
+      </c>
+      <c r="B37" t="s">
         <v>225</v>
       </c>
-      <c r="B37" t="s">
-        <v>226</v>
-      </c>
       <c r="C37" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D37" s="34" t="s">
         <v>125</v>
@@ -2585,10 +2585,10 @@
         <v>4</v>
       </c>
       <c r="H37" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I37" t="s">
         <v>227</v>
-      </c>
-      <c r="I37" t="s">
-        <v>228</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>125</v>
@@ -2599,13 +2599,13 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C38" t="s">
         <v>229</v>
-      </c>
-      <c r="B38" t="s">
-        <v>233</v>
-      </c>
-      <c r="C38" t="s">
-        <v>230</v>
       </c>
       <c r="D38" s="34" t="s">
         <v>125</v>
@@ -2620,10 +2620,10 @@
         <v>4</v>
       </c>
       <c r="H38" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I38" t="s">
         <v>231</v>
-      </c>
-      <c r="I38" t="s">
-        <v>232</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>125</v>
@@ -2634,13 +2634,13 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>233</v>
+      </c>
+      <c r="B39" t="s">
         <v>234</v>
       </c>
-      <c r="B39" t="s">
-        <v>235</v>
-      </c>
       <c r="C39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>125</v>
@@ -2655,10 +2655,10 @@
         <v>3</v>
       </c>
       <c r="H39" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I39" t="s">
         <v>236</v>
-      </c>
-      <c r="I39" t="s">
-        <v>237</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>125</v>
@@ -2706,13 +2706,13 @@
         <v>140</v>
       </c>
       <c r="I41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J41" s="1">
         <v>37</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2741,13 +2741,13 @@
         <v>141</v>
       </c>
       <c r="I42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J42" s="1">
         <v>38</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2767,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>125</v>
@@ -2776,13 +2776,13 @@
         <v>142</v>
       </c>
       <c r="I43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J43" s="1">
         <v>41</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2802,7 +2802,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G44" s="6">
         <v>4</v>
@@ -2811,13 +2811,13 @@
         <v>143</v>
       </c>
       <c r="I44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J44" s="1">
         <v>42</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2846,48 +2846,48 @@
         <v>144</v>
       </c>
       <c r="I45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J45" s="1">
         <v>52</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C46" t="s">
         <v>125</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E46" s="5">
         <v>3</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G46" s="6">
         <v>4</v>
       </c>
       <c r="H46" t="s">
-        <v>149</v>
+        <v>250</v>
       </c>
       <c r="I46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J46" s="1">
         <v>36</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2907,7 +2907,7 @@
         <v>125</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>125</v>
@@ -2916,7 +2916,7 @@
         <v>145</v>
       </c>
       <c r="I47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>125</v>
@@ -2942,7 +2942,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>125</v>
@@ -2951,7 +2951,7 @@
         <v>146</v>
       </c>
       <c r="I48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>125</v>
@@ -2977,7 +2977,7 @@
         <v>125</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>125</v>
@@ -2986,7 +2986,7 @@
         <v>147</v>
       </c>
       <c r="I49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>125</v>
@@ -3021,7 +3021,7 @@
         <v>148</v>
       </c>
       <c r="I50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Update pins such that left/right were swapped to make layout easy
</commit_message>
<xml_diff>
--- a/LayerOne_2014/badge/doc/fpga_pins.xlsx
+++ b/LayerOne_2014/badge/doc/fpga_pins.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="252">
   <si>
     <t>Pin</t>
   </si>
@@ -756,9 +756,6 @@
     <t>P14</t>
   </si>
   <si>
-    <t>P17</t>
-  </si>
-  <si>
     <t>P21</t>
   </si>
   <si>
@@ -769,6 +766,12 @@
   </si>
   <si>
     <t>FPGA_NINIT</t>
+  </si>
+  <si>
+    <t>P65</t>
+  </si>
+  <si>
+    <t>P68</t>
   </si>
 </sst>
 </file>
@@ -1366,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,10 +1812,10 @@
         <v>4</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="G15" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H15" t="s">
         <v>110</v>
@@ -1844,10 +1847,10 @@
         <v>4</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>213</v>
+        <v>16</v>
       </c>
       <c r="G16" s="6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H16" t="s">
         <v>202</v>
@@ -1879,10 +1882,10 @@
         <v>4</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="G17" s="6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>204</v>
@@ -2019,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="G21" s="6">
         <v>2</v>
@@ -2054,10 +2057,10 @@
         <v>4</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>53</v>
+        <v>245</v>
       </c>
       <c r="G22" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>107</v>
@@ -2159,10 +2162,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="G25" s="6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>185</v>
@@ -2194,10 +2197,10 @@
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="G26" s="6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>186</v>
@@ -2229,10 +2232,10 @@
         <v>1</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G27" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>187</v>
@@ -2264,10 +2267,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>217</v>
+        <v>251</v>
       </c>
       <c r="G28" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>188</v>
@@ -2299,10 +2302,10 @@
         <v>1</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>246</v>
+        <v>53</v>
       </c>
       <c r="G29" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>189</v>
@@ -2334,10 +2337,10 @@
         <v>1</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G30" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>190</v>
@@ -2404,10 +2407,10 @@
         <v>2</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>4</v>
+        <v>216</v>
       </c>
       <c r="G32" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>178</v>
@@ -2439,10 +2442,10 @@
         <v>5</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="G33" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>177</v>
@@ -2474,10 +2477,10 @@
         <v>5</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>6</v>
+        <v>212</v>
       </c>
       <c r="G34" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>176</v>
@@ -2509,10 +2512,10 @@
         <v>5</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G35" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>175</v>
@@ -2649,10 +2652,10 @@
         <v>125</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>16</v>
+        <v>246</v>
       </c>
       <c r="G39" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>235</v>
@@ -2872,13 +2875,13 @@
         <v>3</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G46" s="6">
         <v>4</v>
       </c>
       <c r="H46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I46" t="s">
         <v>163</v>
@@ -2977,7 +2980,7 @@
         <v>125</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>125</v>

</xml_diff>